<commit_message>
Improved test on variance and added results to excel file.
</commit_message>
<xml_diff>
--- a/R_code/Bates/partial_calibration_results.xlsx
+++ b/R_code/Bates/partial_calibration_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
   <si>
     <t>eurostoxx</t>
   </si>
@@ -87,11 +87,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -214,9 +217,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -246,6 +252,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="174" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -528,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,131 +557,131 @@
       <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="7"/>
-      <c r="K3" s="11" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="10"/>
+      <c r="K3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="13"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
+      <c r="B4" s="17">
         <v>2.657383E-2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="8">
         <f>G4^2</f>
         <v>4.6068312006090004E-2</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="17">
         <v>0.2146353</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="17">
         <v>0.1121106</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="8">
         <f>P4^2</f>
         <v>2.3222773056040001E-2</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="17">
         <v>0.1523902</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="Q5" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>2.3755330000000002E-2</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="11">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="12">
         <v>2.6068310000000001E-2</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>8.4534559999999995E-2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="5">
         <v>-0.76996547000000004</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="5">
         <v>9.8108600000000004E-2</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="6">
         <v>-1147.117</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="K6" s="6">
+      <c r="I6" s="6"/>
+      <c r="K6" s="9">
         <v>0.11277384</v>
       </c>
       <c r="L6" s="1">
         <v>0.51908628999999995</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="7">
         <v>2.322277E-2</v>
       </c>
       <c r="N6">
@@ -689,19 +698,19 @@
       <c r="B7" s="1">
         <v>2.375495E-2</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="7">
         <v>4.4068309999999999E-2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <v>8.4537769999999998E-2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="5">
         <v>-0.76997863</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="5">
         <v>9.8108619999999994E-2</v>
       </c>
       <c r="H7">
@@ -712,19 +721,19 @@
       <c r="B8" s="1">
         <v>2.1920499999999999E-2</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="7">
         <v>0.02</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="7">
         <v>4.4068309999999999E-2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <v>0.10094754</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="5">
         <v>-0.81809684999999999</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="5">
         <v>9.990462E-2</v>
       </c>
       <c r="H8">
@@ -735,16 +744,16 @@
       <c r="B10">
         <v>3.4290000000000001E-2</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="7">
         <v>2</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="7">
         <v>0</v>
       </c>
       <c r="E10">
         <v>5.2699999999999997E-2</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="7">
         <v>-1</v>
       </c>
       <c r="G10">
@@ -756,22 +765,22 @@
       <c r="K10">
         <v>0.12683</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="7">
         <v>2</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="7">
         <v>0</v>
       </c>
       <c r="N10">
         <v>0.1898629</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="7">
         <v>-1</v>
       </c>
       <c r="P10">
         <v>0.16368669999999999</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="9">
         <v>-2048.65</v>
       </c>
       <c r="R10" t="s">
@@ -782,43 +791,43 @@
       <c r="B11">
         <v>3.4279999999999998E-2</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="7">
         <v>2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="7">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="5">
         <v>5.28E-2</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="13">
         <v>-1</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="6">
         <v>0.157</v>
       </c>
       <c r="I11" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="9">
         <v>0.1290396</v>
       </c>
       <c r="L11">
         <v>3.729562</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="7">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="N11">
         <v>0.21228530000000001</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="7">
         <v>-1</v>
       </c>
       <c r="P11">
         <v>0.18618699999999999</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="9">
         <v>-2055.085</v>
       </c>
     </row>
@@ -829,19 +838,19 @@
       <c r="C13">
         <v>2.3733482600000002</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="5">
         <v>5.9279579999999998E-2</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="7">
         <v>-1</v>
       </c>
       <c r="G13">
         <v>0.16854503000000001</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="9">
         <v>-1266.386</v>
       </c>
       <c r="I13" t="s">
@@ -887,7 +896,7 @@
       <c r="L17">
         <v>36.6</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="4">
         <v>2.4600000000000002E-5</v>
       </c>
       <c r="N17">
@@ -907,7 +916,7 @@
       <c r="D18">
         <v>2.6400000000000001E-5</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="5">
         <v>7.1040000000000006E-2</v>
       </c>
       <c r="J18" t="s">
@@ -956,6 +965,68 @@
       </c>
       <c r="N19">
         <v>4.8480000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="9">
+        <v>48.393621646</v>
+      </c>
+      <c r="D21">
+        <v>9.1574129999999997E-3</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1.331405878</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="9">
+        <v>55.711931460000002</v>
+      </c>
+      <c r="D22" s="3">
+        <v>5.7750290000000001E-3</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1.134439089</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="9">
+        <v>64.844488952000006</v>
+      </c>
+      <c r="D23">
+        <v>2.759109E-3</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.84596213200000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="20">
+        <v>24.26512</v>
+      </c>
+      <c r="D25" s="2">
+        <v>9.2551969999999999E-4</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1.611847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New results and bug fixing, results are unsatisfactory.
</commit_message>
<xml_diff>
--- a/R_code/Bates/partial_calibration_results.xlsx
+++ b/R_code/Bates/partial_calibration_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
   <si>
     <t>eurostoxx</t>
   </si>
@@ -81,6 +81,27 @@
   </si>
   <si>
     <t>sampled value</t>
+  </si>
+  <si>
+    <t>vasicek</t>
+  </si>
+  <si>
+    <t>eur/usd</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>ha due ben distinti trend</t>
+  </si>
+  <si>
+    <t>sample vol</t>
+  </si>
+  <si>
+    <t>sample var</t>
+  </si>
+  <si>
+    <t>sample mu</t>
   </si>
 </sst>
 </file>
@@ -94,7 +115,7 @@
     <numFmt numFmtId="167" formatCode="0.00000000"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -217,7 +238,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -236,6 +257,13 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -246,15 +274,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -537,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,492 +584,935 @@
     <col min="2" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="9" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="8" max="10" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="G1" s="20"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="10"/>
-      <c r="K3" s="14" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="K3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="16"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="17">
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="19"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="14">
         <v>2.657383E-2</v>
       </c>
-      <c r="D4" s="8">
-        <f>G4^2</f>
+      <c r="D5" s="8">
+        <f>G5^2</f>
         <v>4.6068312006090004E-2</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G5" s="14">
         <v>0.2146353</v>
       </c>
-      <c r="K4" s="17">
+      <c r="L5" s="14">
         <v>0.1121106</v>
       </c>
-      <c r="M4" s="8">
-        <f>P4^2</f>
+      <c r="N5" s="8">
+        <f>Q5^2</f>
         <v>2.3222773056040001E-2</v>
       </c>
-      <c r="P4" s="17">
+      <c r="Q5" s="14">
         <v>0.1523902</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="M6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="N6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="O6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="P6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="Q6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="R6" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
         <v>2.3755330000000002E-2</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C7" s="11">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D7" s="12">
         <v>2.6068310000000001E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E7" s="5">
         <v>8.4534559999999995E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F7" s="5">
         <v>-0.76996547000000004</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G7" s="5">
         <v>9.8108600000000004E-2</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H7" s="6">
         <v>-1147.117</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="K6" s="9">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="L7" s="9">
         <v>0.11277384</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M7" s="1">
         <v>0.51908628999999995</v>
       </c>
-      <c r="M6" s="7">
+      <c r="N7" s="7">
         <v>2.322277E-2</v>
       </c>
-      <c r="N6">
+      <c r="O7">
         <v>1.1417539699999999</v>
       </c>
-      <c r="O6">
+      <c r="P7">
         <v>-0.94884714000000003</v>
       </c>
-      <c r="P6">
+      <c r="Q7">
         <v>0.31580809999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
         <v>2.375495E-2</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="7">
         <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="D7" s="7">
-        <v>4.4068309999999999E-2</v>
-      </c>
-      <c r="E7" s="5">
-        <v>8.4537769999999998E-2</v>
-      </c>
-      <c r="F7" s="5">
-        <v>-0.76997863</v>
-      </c>
-      <c r="G7" s="5">
-        <v>9.8108619999999994E-2</v>
-      </c>
-      <c r="H7">
-        <v>-1147.1130000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>2.1920499999999999E-2</v>
-      </c>
-      <c r="C8" s="7">
-        <v>0.02</v>
       </c>
       <c r="D8" s="7">
         <v>4.4068309999999999E-2</v>
       </c>
       <c r="E8" s="5">
+        <v>8.4537769999999998E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>-0.76997863</v>
+      </c>
+      <c r="G8" s="5">
+        <v>9.8108619999999994E-2</v>
+      </c>
+      <c r="H8">
+        <v>-1147.1130000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>2.1920499999999999E-2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4.4068309999999999E-2</v>
+      </c>
+      <c r="E9" s="5">
         <v>0.10094754</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F9" s="5">
         <v>-0.81809684999999999</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G9" s="5">
         <v>9.990462E-2</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>-1127.9000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>3.4290000000000001E-2</v>
-      </c>
-      <c r="C10" s="7">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>5.2699999999999997E-2</v>
-      </c>
-      <c r="F10" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G10">
-        <v>0.157</v>
-      </c>
-      <c r="I10" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10">
-        <v>0.12683</v>
-      </c>
-      <c r="L10" s="7">
-        <v>2</v>
-      </c>
-      <c r="M10" s="7">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0.1898629</v>
-      </c>
-      <c r="O10" s="7">
-        <v>-1</v>
-      </c>
-      <c r="P10">
-        <v>0.16368669999999999</v>
-      </c>
-      <c r="Q10" s="9">
-        <v>-2048.65</v>
-      </c>
-      <c r="R10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>3.4279999999999998E-2</v>
       </c>
       <c r="C11" s="7">
         <v>2</v>
       </c>
       <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G11">
+        <v>0.157</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>0.12683</v>
+      </c>
+      <c r="M11" s="7">
+        <v>2</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0.1898629</v>
+      </c>
+      <c r="P11" s="7">
+        <v>-1</v>
+      </c>
+      <c r="Q11">
+        <v>0.16368669999999999</v>
+      </c>
+      <c r="R11" s="9">
+        <v>-2048.65</v>
+      </c>
+      <c r="S11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3.4279999999999998E-2</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E12" s="5">
         <v>5.28E-2</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F12" s="13">
         <v>-1</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G12" s="6">
         <v>0.157</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="9">
+      <c r="L12" s="9">
         <v>0.1290396</v>
       </c>
-      <c r="L11">
+      <c r="M12">
         <v>3.729562</v>
       </c>
-      <c r="M11" s="7">
+      <c r="N12" s="7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="N11">
+      <c r="O12">
         <v>0.21228530000000001</v>
       </c>
-      <c r="O11" s="7">
+      <c r="P12" s="7">
         <v>-1</v>
       </c>
-      <c r="P11">
+      <c r="Q12">
         <v>0.18618699999999999</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="R12" s="9">
         <v>-2055.085</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B14">
         <v>3.4445509999999999E-2</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>2.3733482600000002</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D14" s="7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E14" s="5">
         <v>5.9279579999999998E-2</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F14" s="7">
         <v>-1</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>0.16854503000000001</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H14" s="9">
         <v>-1266.386</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K17" t="s">
         <v>13</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="M17" s="21"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C17">
-        <v>48.3</v>
-      </c>
-      <c r="D17">
-        <v>3.5899999999999998E-5</v>
-      </c>
-      <c r="E17">
-        <v>8.3299999999999999E-2</v>
-      </c>
-      <c r="J17" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="C18" s="9">
+        <v>48.393621646</v>
+      </c>
+      <c r="D18">
+        <v>9.1574129999999997E-3</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1.331405878</v>
+      </c>
+      <c r="K18" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" t="s">
         <v>17</v>
       </c>
-      <c r="L17">
-        <v>36.6</v>
-      </c>
-      <c r="M17" s="4">
-        <v>2.4600000000000002E-5</v>
-      </c>
-      <c r="N17">
-        <v>6.012E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18">
-        <v>55.7</v>
-      </c>
-      <c r="D18">
-        <v>2.6400000000000001E-5</v>
-      </c>
-      <c r="E18" s="5">
-        <v>7.1040000000000006E-2</v>
-      </c>
-      <c r="J18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18">
-        <v>63.3</v>
-      </c>
-      <c r="M18">
-        <v>1.164E-5</v>
-      </c>
-      <c r="N18">
-        <v>5.4339999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M18" s="9">
+        <v>36.682249927999997</v>
+      </c>
+      <c r="N18" s="4">
+        <v>6.2823469999999998E-3</v>
+      </c>
+      <c r="O18">
+        <v>0.96010544799999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="9">
+        <v>46.290590000000002</v>
+      </c>
+      <c r="D19" s="3">
+        <v>6.9503899999999999E-3</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.134439089</v>
+      </c>
+      <c r="K19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="9">
+        <v>38.608978</v>
+      </c>
+      <c r="N19">
+        <v>4.8759770000000001E-3</v>
+      </c>
+      <c r="O19">
+        <v>0.86777000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="C19">
-        <v>64.8</v>
-      </c>
-      <c r="D19">
-        <v>1.08E-5</v>
-      </c>
-      <c r="E19">
-        <v>5.2900000000000003E-2</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="C20" s="9">
+        <v>8.8474579999999996</v>
+      </c>
+      <c r="D20">
+        <v>4.8147579999999997E-3</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.41278700000000002</v>
+      </c>
+      <c r="K20" t="s">
         <v>16</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L20" t="s">
         <v>16</v>
       </c>
-      <c r="L19">
-        <v>55.3</v>
-      </c>
-      <c r="M19">
-        <v>1.062E-5</v>
-      </c>
-      <c r="N19">
-        <v>4.8480000000000002E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="M20" s="9">
+        <v>11.11538</v>
+      </c>
+      <c r="N20">
+        <v>3.2098970000000002E-3</v>
+      </c>
+      <c r="O20">
+        <v>0.37777888900000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="E21" s="5"/>
+      <c r="M21" s="21"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="16">
+        <v>24.26512</v>
+      </c>
+      <c r="D23" s="9">
+        <v>4.7201510000000002E-2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1.611847</v>
+      </c>
+      <c r="K23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23" s="9">
+        <v>19.986193539999999</v>
+      </c>
+      <c r="N23">
+        <v>2.320345E-2</v>
+      </c>
+      <c r="O23">
+        <v>1.52370239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="9">
+        <v>3.8436575999999998</v>
+      </c>
+      <c r="D24">
+        <v>4.692321E-2</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.53759599999999996</v>
+      </c>
+      <c r="K24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" s="9">
+        <v>6.1586889999999999</v>
+      </c>
+      <c r="N24">
+        <v>2.3133379999999999E-2</v>
+      </c>
+      <c r="O24">
+        <v>0.63388865000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="K29" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="19"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="14">
+        <v>-2.5284979999999999E-2</v>
+      </c>
+      <c r="D31" s="8">
+        <f>G31^2</f>
+        <v>8.3608657825729009E-3</v>
+      </c>
+      <c r="G31" s="14">
+        <v>9.1437770000000002E-2</v>
+      </c>
+      <c r="L31" s="14">
+        <v>3.2958750000000002E-3</v>
+      </c>
+      <c r="N31" s="8">
+        <f>Q31^2</f>
+        <v>2.945383628944E-2</v>
+      </c>
+      <c r="Q31" s="14">
+        <v>0.1716212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="P32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q32" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="R32" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="9">
+        <v>-2.6980474000000001E-2</v>
+      </c>
+      <c r="C33">
+        <v>0.61766291500000003</v>
+      </c>
+      <c r="D33" s="22">
+        <v>8.1608649999999998E-3</v>
+      </c>
+      <c r="E33">
+        <v>0.39102463700000001</v>
+      </c>
+      <c r="F33">
+        <v>-0.99084982200000005</v>
+      </c>
+      <c r="G33">
+        <v>0.20107651100000001</v>
+      </c>
+      <c r="H33" s="9">
+        <v>-1913.6880000000001</v>
+      </c>
+      <c r="L33" s="25">
+        <v>6.8859050000000005E-2</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0.40454250000000003</v>
+      </c>
+      <c r="N33">
+        <v>3.1989919999999998E-2</v>
+      </c>
+      <c r="O33" s="26">
+        <v>1.000001E-5</v>
+      </c>
+      <c r="P33" s="2">
+        <v>-0.2552545</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>0.1588503</v>
+      </c>
+      <c r="R33">
+        <v>-79.11</v>
+      </c>
+      <c r="T33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="9">
+        <v>-1.520226E-2</v>
+      </c>
+      <c r="C34">
+        <v>1.5099327600000001</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E34">
+        <v>0.20654532</v>
+      </c>
+      <c r="F34" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G34">
+        <v>0.16263025</v>
+      </c>
+      <c r="H34">
+        <v>-1985.4480000000001</v>
+      </c>
+      <c r="I34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L34" s="9">
+        <v>-7.2084049999999997E-2</v>
+      </c>
+      <c r="M34" s="7">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>1.369982E-2</v>
+      </c>
+      <c r="O34">
+        <v>0.78661219999999998</v>
+      </c>
+      <c r="P34">
+        <v>-0.97991225000000004</v>
+      </c>
+      <c r="Q34">
+        <v>0.62051568000000001</v>
+      </c>
+      <c r="R34">
+        <v>-497.94</v>
+      </c>
+      <c r="S34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="9">
-        <v>48.393621646</v>
-      </c>
-      <c r="D21">
-        <v>9.1574129999999997E-3</v>
-      </c>
-      <c r="E21" s="5">
-        <v>1.331405878</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="9">
-        <v>55.711931460000002</v>
-      </c>
-      <c r="D22" s="3">
-        <v>5.7750290000000001E-3</v>
-      </c>
-      <c r="E22" s="5">
-        <v>1.134439089</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C39" s="24">
+        <v>70.007299959999997</v>
+      </c>
+      <c r="D39">
+        <v>1.2128900000000001E-3</v>
+      </c>
+      <c r="E39">
+        <v>0.58279024999999995</v>
+      </c>
+      <c r="K39" t="s">
+        <v>15</v>
+      </c>
+      <c r="L39" t="s">
+        <v>17</v>
+      </c>
+      <c r="M39" s="9">
+        <v>68.903152410999994</v>
+      </c>
+      <c r="N39" s="21">
+        <v>5.6944639999999998E-3</v>
+      </c>
+      <c r="O39" s="21">
+        <v>1.2527833239999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="24">
+        <v>59.21</v>
+      </c>
+      <c r="D40">
+        <v>9.1889999999999995E-4</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.46654699999999999</v>
+      </c>
+      <c r="K40" t="s">
+        <v>15</v>
+      </c>
+      <c r="L40" t="s">
+        <v>15</v>
+      </c>
+      <c r="M40" s="9">
+        <v>36.626773122000003</v>
+      </c>
+      <c r="N40" s="21">
+        <v>6.8433239999999996E-3</v>
+      </c>
+      <c r="O40" s="21">
+        <v>1.0012969229999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>16</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B41" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="9">
-        <v>64.844488952000006</v>
-      </c>
-      <c r="D23">
-        <v>2.759109E-3</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0.84596213200000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="20">
-        <v>24.26512</v>
-      </c>
-      <c r="D25" s="2">
-        <v>9.2551969999999999E-4</v>
-      </c>
-      <c r="E25" s="5">
-        <v>1.611847</v>
+      <c r="C41" s="24">
+        <v>7.0909684999999998</v>
+      </c>
+      <c r="D41">
+        <v>5.9630000000000002E-4</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.13006000000000001</v>
+      </c>
+      <c r="K41" t="s">
+        <v>16</v>
+      </c>
+      <c r="L41" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="9">
+        <v>13.86</v>
+      </c>
+      <c r="N41" s="21">
+        <v>2.7753729999999998E-3</v>
+      </c>
+      <c r="O41" s="21">
+        <v>0.39228393900000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="21"/>
+      <c r="K43" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="9">
+        <v>34.126119142</v>
+      </c>
+      <c r="D44">
+        <v>7.9834780000000004E-3</v>
+      </c>
+      <c r="E44">
+        <v>0.56086166400000004</v>
+      </c>
+      <c r="K44" t="s">
+        <v>15</v>
+      </c>
+      <c r="L44" t="s">
+        <v>15</v>
+      </c>
+      <c r="M44" s="9">
+        <v>37.993173689999999</v>
+      </c>
+      <c r="N44" s="21">
+        <v>2.9184760000000001E-2</v>
+      </c>
+      <c r="O44" s="21">
+        <v>1.6369652299999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45">
+        <v>4.3243999999999998</v>
+      </c>
+      <c r="D45">
+        <v>8.1299000000000007E-3</v>
+      </c>
+      <c r="E45">
+        <v>0.1517</v>
+      </c>
+      <c r="K45" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" t="s">
+        <v>16</v>
+      </c>
+      <c r="M45" s="9">
+        <v>7.2202380000000002</v>
+      </c>
+      <c r="N45" s="21">
+        <v>3.0728829999999999E-2</v>
+      </c>
+      <c r="O45" s="21">
+        <v>0.56113345000000003</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="K3:Q3"/>
+  <mergeCells count="5">
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="K29:S29"/>
+    <mergeCell ref="K3:S3"/>
+    <mergeCell ref="A3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added results and comments, final commit of the day.
</commit_message>
<xml_diff>
--- a/R_code/Bates/partial_calibration_results.xlsx
+++ b/R_code/Bates/partial_calibration_results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="30">
   <si>
     <t>eurostoxx</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>sample mu</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>locked from vasicek monthly</t>
+  </si>
+  <si>
+    <t>potrebbe avere senso: k=0 per spiegare tutta la volatilità in modo stocatico dato che anche il rendimento medio è quasi nullo</t>
+  </si>
+  <si>
+    <t>locked from vasicek monthly, k0=0.4</t>
   </si>
 </sst>
 </file>
@@ -117,7 +129,7 @@
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +165,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,8 +198,18 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -232,16 +269,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -254,9 +355,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -277,22 +375,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,40 +720,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-      <c r="K3" s="17" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="K3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="19"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="15"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -635,8 +768,8 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
       <c r="L4" t="s">
         <v>25</v>
       </c>
@@ -648,201 +781,266 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>2.657383E-2</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <f>G5^2</f>
         <v>4.6068312006090004E-2</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="10">
         <v>0.2146353</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="10">
         <v>0.1121106</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <f>Q5^2</f>
         <v>2.3222773056040001E-2</v>
       </c>
-      <c r="Q5" s="14">
+      <c r="Q5" s="10">
         <v>0.1523902</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="R6" s="15" t="s">
+      <c r="R6" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
+      <c r="B7" s="22">
         <v>2.3755330000000002E-2</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="23">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="24">
         <v>2.6068310000000001E-2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="22">
         <v>8.4534559999999995E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="22">
         <v>-0.76996547000000004</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="22">
         <v>9.8108600000000004E-2</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="25">
         <v>-1147.117</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="L7" s="9">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="L7" s="35">
         <v>0.11277384</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="36">
         <v>0.51908628999999995</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="37">
         <v>2.322277E-2</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="38">
         <v>1.1417539699999999</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="38">
         <v>-0.94884714000000003</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="38">
         <v>0.31580809999999998</v>
       </c>
+      <c r="R7" s="38"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+      <c r="B8" s="26">
         <v>2.375495E-2</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="27">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="28">
         <v>4.4068309999999999E-2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="29">
         <v>8.4537769999999998E-2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="29">
         <v>-0.76997863</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="29">
         <v>9.8108619999999994E-2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="30">
         <v>-1147.1130000000001</v>
       </c>
+      <c r="L8" s="34">
+        <v>0.11277065</v>
+      </c>
+      <c r="M8" s="30">
+        <v>0.52321364000000004</v>
+      </c>
+      <c r="N8" s="28">
+        <v>2.3033379999999999E-2</v>
+      </c>
+      <c r="O8" s="30">
+        <v>1.1401397</v>
+      </c>
+      <c r="P8" s="30">
+        <v>-0.94897178999999998</v>
+      </c>
+      <c r="Q8" s="30">
+        <v>0.31570431999999998</v>
+      </c>
+      <c r="R8" s="34">
+        <v>-1862.65</v>
+      </c>
+      <c r="S8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
+      <c r="B9" s="26">
         <v>2.1920499999999999E-2</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="27">
         <v>0.02</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="28">
         <v>4.4068309999999999E-2</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="29">
         <v>0.10094754</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="29">
         <v>-0.81809684999999999</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="29">
         <v>9.990462E-2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="30">
         <v>-1127.9000000000001</v>
       </c>
+      <c r="L9" s="34">
+        <v>0.11249726</v>
+      </c>
+      <c r="M9" s="30">
+        <v>0.29393791000000002</v>
+      </c>
+      <c r="N9" s="28">
+        <v>2.3033379999999999E-2</v>
+      </c>
+      <c r="O9" s="28">
+        <v>0.63398865000000004</v>
+      </c>
+      <c r="P9" s="30">
+        <v>-0.94947121000000001</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>0.23828381000000001</v>
+      </c>
+      <c r="R9" s="39">
+        <v>-1852.09</v>
+      </c>
+      <c r="S9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="30">
+        <v>2.3968110000000001E-2</v>
+      </c>
+      <c r="C10" s="27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D10" s="28">
+        <v>4.6913200000000002E-2</v>
+      </c>
+      <c r="E10" s="28">
+        <v>0.10577300000000001</v>
+      </c>
+      <c r="F10" s="30">
+        <v>-0.75877607000000002</v>
+      </c>
+      <c r="G10" s="30">
+        <v>0.10519911</v>
+      </c>
+      <c r="H10" s="30">
+        <v>-1140.8910000000001</v>
+      </c>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>3.4290000000000001E-2</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="L11" s="30">
+        <v>0.12683</v>
+      </c>
+      <c r="M11" s="27">
         <v>2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="N11" s="27">
         <v>0</v>
       </c>
-      <c r="E11">
-        <v>5.2699999999999997E-2</v>
-      </c>
-      <c r="F11" s="7">
+      <c r="O11" s="30">
+        <v>0.1898629</v>
+      </c>
+      <c r="P11" s="27">
         <v>-1</v>
       </c>
-      <c r="G11">
-        <v>0.157</v>
-      </c>
-      <c r="I11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11">
-        <v>0.12683</v>
-      </c>
-      <c r="M11" s="7">
-        <v>2</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0.1898629</v>
-      </c>
-      <c r="P11" s="7">
-        <v>-1</v>
-      </c>
-      <c r="Q11">
+      <c r="Q11" s="30">
         <v>0.16368669999999999</v>
       </c>
-      <c r="R11" s="9">
+      <c r="R11" s="34">
         <v>-2048.65</v>
       </c>
       <c r="S11" t="s">
@@ -850,74 +1048,129 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="B12" s="30">
+        <v>3.4290000000000001E-2</v>
+      </c>
+      <c r="C12" s="27">
+        <v>2</v>
+      </c>
+      <c r="D12" s="27">
+        <v>0</v>
+      </c>
+      <c r="E12" s="30">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="F12" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="30">
+        <v>0.157</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="34">
+        <v>0.1290396</v>
+      </c>
+      <c r="M12" s="30">
+        <v>3.729562</v>
+      </c>
+      <c r="N12" s="27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="O12" s="30">
+        <v>0.21228530000000001</v>
+      </c>
+      <c r="P12" s="27">
+        <v>-1</v>
+      </c>
+      <c r="Q12" s="30">
+        <v>0.18618699999999999</v>
+      </c>
+      <c r="R12" s="34">
+        <v>-2055.085</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="30">
         <v>3.4279999999999998E-2</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C13" s="27">
         <v>2</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D13" s="27">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E13" s="29">
         <v>5.28E-2</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F13" s="31">
         <v>-1</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G13" s="32">
         <v>0.157</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="9">
-        <v>0.1290396</v>
-      </c>
-      <c r="M12">
-        <v>3.729562</v>
-      </c>
-      <c r="N12" s="7">
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="30">
+        <v>3.4445509999999999E-2</v>
+      </c>
+      <c r="C15" s="33">
+        <v>2.3733482600000002</v>
+      </c>
+      <c r="D15" s="27">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="O12">
-        <v>0.21228530000000001</v>
-      </c>
-      <c r="P12" s="7">
+      <c r="E15" s="29">
+        <v>5.9279579999999998E-2</v>
+      </c>
+      <c r="F15" s="27">
         <v>-1</v>
       </c>
-      <c r="Q12">
-        <v>0.18618699999999999</v>
-      </c>
-      <c r="R12" s="9">
-        <v>-2055.085</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>3.4445509999999999E-2</v>
-      </c>
-      <c r="C14">
-        <v>2.3733482600000002</v>
-      </c>
-      <c r="D14" s="7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="E14" s="5">
-        <v>5.9279579999999998E-2</v>
-      </c>
-      <c r="F14" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G14">
+      <c r="G15" s="30">
         <v>0.16854503000000001</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H15" s="34">
         <v>-1266.386</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" t="s">
         <v>9</v>
       </c>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -932,7 +1185,7 @@
       <c r="L17" t="s">
         <v>14</v>
       </c>
-      <c r="M17" s="21"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -941,13 +1194,13 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>48.393621646</v>
       </c>
       <c r="D18">
         <v>9.1574129999999997E-3</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>1.331405878</v>
       </c>
       <c r="K18" t="s">
@@ -956,10 +1209,10 @@
       <c r="L18" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="8">
         <v>36.682249927999997</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18" s="3">
         <v>6.2823469999999998E-3</v>
       </c>
       <c r="O18">
@@ -973,13 +1226,13 @@
       <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>46.290590000000002</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>6.9503899999999999E-3</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>1.134439089</v>
       </c>
       <c r="K19" t="s">
@@ -988,7 +1241,7 @@
       <c r="L19" t="s">
         <v>15</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="8">
         <v>38.608978</v>
       </c>
       <c r="N19">
@@ -1005,13 +1258,13 @@
       <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>8.8474579999999996</v>
       </c>
       <c r="D20">
         <v>4.8147579999999997E-3</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>0.41278700000000002</v>
       </c>
       <c r="K20" t="s">
@@ -1020,7 +1273,7 @@
       <c r="L20" t="s">
         <v>16</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="8">
         <v>11.11538</v>
       </c>
       <c r="N20">
@@ -1031,15 +1284,15 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C21" s="9"/>
-      <c r="E21" s="5"/>
-      <c r="M21" s="21"/>
+      <c r="C21" s="8"/>
+      <c r="E21" s="4"/>
+      <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="K22" s="27" t="s">
+      <c r="K22" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1050,13 +1303,13 @@
       <c r="B23" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="12">
         <v>24.26512</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>4.7201510000000002E-2</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>1.611847</v>
       </c>
       <c r="K23" t="s">
@@ -1065,7 +1318,7 @@
       <c r="L23" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="8">
         <v>19.986193539999999</v>
       </c>
       <c r="N23">
@@ -1082,13 +1335,13 @@
       <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>3.8436575999999998</v>
       </c>
       <c r="D24">
         <v>4.692321E-2</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>0.53759599999999996</v>
       </c>
       <c r="K24" t="s">
@@ -1097,7 +1350,7 @@
       <c r="L24" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M24" s="8">
         <v>6.1586889999999999</v>
       </c>
       <c r="N24">
@@ -1108,28 +1361,28 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="19"/>
-      <c r="K29" s="17" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
+      <c r="K29" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="19"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="15"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -1152,112 +1405,112 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="14">
+      <c r="B31" s="10">
         <v>-2.5284979999999999E-2</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <f>G31^2</f>
         <v>8.3608657825729009E-3</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="10">
         <v>9.1437770000000002E-2</v>
       </c>
-      <c r="L31" s="14">
+      <c r="L31" s="10">
         <v>3.2958750000000002E-3</v>
       </c>
-      <c r="N31" s="8">
+      <c r="N31" s="7">
         <f>Q31^2</f>
         <v>2.945383628944E-2</v>
       </c>
-      <c r="Q31" s="14">
+      <c r="Q31" s="10">
         <v>0.1716212</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="15" t="s">
+      <c r="G32" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="L32" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="M32" s="15" t="s">
+      <c r="M32" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N32" s="15" t="s">
+      <c r="N32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O32" s="15" t="s">
+      <c r="O32" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="P32" s="15" t="s">
+      <c r="P32" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Q32" s="15" t="s">
+      <c r="Q32" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="R32" s="15" t="s">
+      <c r="R32" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="9">
+      <c r="B33" s="35">
         <v>-2.6980474000000001E-2</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="38">
         <v>0.61766291500000003</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="40">
         <v>8.1608649999999998E-3</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="38">
         <v>0.39102463700000001</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="38">
         <v>-0.99084982200000005</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="38">
         <v>0.20107651100000001</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="35">
         <v>-1913.6880000000001</v>
       </c>
-      <c r="L33" s="25">
+      <c r="L33" s="42">
         <v>6.8859050000000005E-2</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="43">
         <v>0.40454250000000003</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="38">
         <v>3.1989919999999998E-2</v>
       </c>
-      <c r="O33" s="26">
+      <c r="O33" s="44">
         <v>1.000001E-5</v>
       </c>
-      <c r="P33" s="2">
+      <c r="P33" s="43">
         <v>-0.2552545</v>
       </c>
-      <c r="Q33" s="2">
+      <c r="Q33" s="43">
         <v>0.1588503</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="25">
         <v>-79.11</v>
       </c>
       <c r="T33" t="s">
@@ -1265,244 +1518,389 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="9">
+      <c r="B34" s="34">
         <v>-1.520226E-2</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="30">
         <v>1.5099327600000001</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="27">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="30">
         <v>0.20654532</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="27">
         <v>-1</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="30">
         <v>0.16263025</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="30">
         <v>-1985.4480000000001</v>
       </c>
       <c r="I34" t="s">
         <v>9</v>
       </c>
-      <c r="L34" s="9">
+      <c r="L34" s="34">
         <v>-7.2084049999999997E-2</v>
       </c>
-      <c r="M34" s="7">
+      <c r="M34" s="27">
         <v>0</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="30">
         <v>1.369982E-2</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="30">
         <v>0.78661219999999998</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="30">
         <v>-0.97991225000000004</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="30">
         <v>0.62051568000000001</v>
       </c>
-      <c r="R34">
+      <c r="R34" s="32">
         <v>-497.94</v>
       </c>
       <c r="S34" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="34">
+        <v>-2.6932873E-2</v>
+      </c>
+      <c r="C35" s="30">
+        <v>0.62024193400000005</v>
+      </c>
+      <c r="D35" s="28">
+        <v>8.0299759999999994E-3</v>
+      </c>
+      <c r="E35" s="30">
+        <v>0.38700683899999999</v>
+      </c>
+      <c r="F35" s="30">
+        <v>-0.99140952800000004</v>
+      </c>
+      <c r="G35" s="30">
+        <v>0.20030995100000001</v>
+      </c>
+      <c r="H35" s="41">
+        <v>-1914.308</v>
+      </c>
+      <c r="I35" t="s">
+        <v>27</v>
+      </c>
+      <c r="L35" s="34">
+        <v>5.9465230000000001E-2</v>
+      </c>
+      <c r="M35" s="27">
+        <v>10</v>
+      </c>
+      <c r="N35" s="28">
+        <v>3.0628829999999999E-2</v>
+      </c>
+      <c r="O35" s="30">
+        <v>0.70060725000000001</v>
+      </c>
+      <c r="P35" s="30">
+        <v>-1</v>
+      </c>
+      <c r="Q35" s="30">
+        <v>0.33561477000000001</v>
+      </c>
+      <c r="R35" s="34">
+        <v>-126.2882</v>
+      </c>
+      <c r="S35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="34">
+        <v>-2.767066E-2</v>
+      </c>
+      <c r="C36" s="30">
+        <v>0.29812903499999999</v>
+      </c>
+      <c r="D36" s="28">
+        <v>8.0299759999999994E-3</v>
+      </c>
+      <c r="E36" s="28">
+        <v>0.15180279999999999</v>
+      </c>
+      <c r="F36" s="30">
+        <v>-1</v>
+      </c>
+      <c r="G36" s="30">
+        <v>0.12748636099999999</v>
+      </c>
+      <c r="H36" s="30">
+        <v>-1836.7190000000001</v>
+      </c>
+      <c r="I36" t="s">
+        <v>27</v>
+      </c>
+      <c r="L36" s="34">
+        <v>-9.6763960000000003E-3</v>
+      </c>
+      <c r="M36" s="45">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="N36" s="28">
+        <v>3.0628826000000001E-2</v>
+      </c>
+      <c r="O36" s="30">
+        <v>2.1042205209999998</v>
+      </c>
+      <c r="P36" s="30">
+        <v>-0.85683910399999996</v>
+      </c>
+      <c r="Q36" s="30">
+        <v>0.59100132599999999</v>
+      </c>
+      <c r="R36" s="34">
+        <v>-945.471</v>
+      </c>
+      <c r="S36" t="s">
+        <v>29</v>
+      </c>
+      <c r="T36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="L37" s="30">
+        <v>-8.2370859999999994E-3</v>
+      </c>
+      <c r="M37" s="27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="N37" s="28">
+        <v>3.0628826000000001E-2</v>
+      </c>
+      <c r="O37" s="28">
+        <v>0.56123345000000002</v>
+      </c>
+      <c r="P37" s="30">
+        <v>-0.81253739599999997</v>
+      </c>
+      <c r="Q37" s="30">
+        <v>0.30387926799999998</v>
+      </c>
+      <c r="R37" s="30">
+        <v>-834.17859999999996</v>
+      </c>
+      <c r="S37" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" t="s">
-        <v>14</v>
-      </c>
-      <c r="K38" t="s">
-        <v>13</v>
-      </c>
-      <c r="L38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="24">
-        <v>70.007299959999997</v>
-      </c>
-      <c r="D39">
-        <v>1.2128900000000001E-3</v>
-      </c>
-      <c r="E39">
-        <v>0.58279024999999995</v>
-      </c>
-      <c r="K39" t="s">
-        <v>15</v>
-      </c>
-      <c r="L39" t="s">
-        <v>17</v>
-      </c>
-      <c r="M39" s="9">
-        <v>68.903152410999994</v>
-      </c>
-      <c r="N39" s="21">
-        <v>5.6944639999999998E-3</v>
-      </c>
-      <c r="O39" s="21">
-        <v>1.2527833239999999</v>
-      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="24">
-        <v>59.21</v>
-      </c>
-      <c r="D40">
-        <v>9.1889999999999995E-4</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0.46654699999999999</v>
+        <v>14</v>
       </c>
       <c r="K40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L40" t="s">
-        <v>15</v>
-      </c>
-      <c r="M40" s="9">
-        <v>36.626773122000003</v>
-      </c>
-      <c r="N40" s="21">
-        <v>6.8433239999999996E-3</v>
-      </c>
-      <c r="O40" s="21">
-        <v>1.0012969229999999</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="19">
+        <v>70.007299959999997</v>
+      </c>
+      <c r="D41">
+        <v>1.2128900000000001E-3</v>
+      </c>
+      <c r="E41">
+        <v>0.58279024999999995</v>
+      </c>
+      <c r="K41" t="s">
+        <v>15</v>
+      </c>
+      <c r="L41" t="s">
+        <v>17</v>
+      </c>
+      <c r="M41" s="8">
+        <v>68.903152410999994</v>
+      </c>
+      <c r="N41" s="17">
+        <v>5.6944639999999998E-3</v>
+      </c>
+      <c r="O41" s="17">
+        <v>1.2527833239999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="19">
+        <v>59.21</v>
+      </c>
+      <c r="D42">
+        <v>9.1889999999999995E-4</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.46654699999999999</v>
+      </c>
+      <c r="K42" t="s">
+        <v>15</v>
+      </c>
+      <c r="L42" t="s">
+        <v>15</v>
+      </c>
+      <c r="M42" s="8">
+        <v>36.626773122000003</v>
+      </c>
+      <c r="N42" s="17">
+        <v>6.8433239999999996E-3</v>
+      </c>
+      <c r="O42" s="17">
+        <v>1.0012969229999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>16</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C43" s="19">
         <v>7.0909684999999998</v>
       </c>
-      <c r="D41">
+      <c r="D43">
         <v>5.9630000000000002E-4</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E43" s="1">
         <v>0.13006000000000001</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K43" t="s">
         <v>16</v>
       </c>
-      <c r="L41" t="s">
+      <c r="L43" t="s">
         <v>16</v>
       </c>
-      <c r="M41" s="9">
+      <c r="M43" s="8">
         <v>13.86</v>
       </c>
-      <c r="N41" s="21">
+      <c r="N43" s="17">
         <v>2.7753729999999998E-3</v>
       </c>
-      <c r="O41" s="21">
+      <c r="O43" s="17">
         <v>0.39228393900000003</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
-      <c r="O42" s="21"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="K43" s="23" t="s">
+      <c r="C45" s="17"/>
+      <c r="K45" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="M43" s="21"/>
-      <c r="N43" s="21"/>
-      <c r="O43" s="21"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>15</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C46" s="8">
         <v>34.126119142</v>
       </c>
-      <c r="D44">
+      <c r="D46">
         <v>7.9834780000000004E-3</v>
       </c>
-      <c r="E44">
+      <c r="E46">
         <v>0.56086166400000004</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K46" t="s">
         <v>15</v>
       </c>
-      <c r="L44" t="s">
+      <c r="L46" t="s">
         <v>15</v>
       </c>
-      <c r="M44" s="9">
+      <c r="M46" s="8">
         <v>37.993173689999999</v>
       </c>
-      <c r="N44" s="21">
+      <c r="N46" s="17">
         <v>2.9184760000000001E-2</v>
       </c>
-      <c r="O44" s="21">
+      <c r="O46" s="17">
         <v>1.6369652299999999</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>16</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>16</v>
       </c>
-      <c r="C45">
+      <c r="C47">
         <v>4.3243999999999998</v>
       </c>
-      <c r="D45">
+      <c r="D47">
         <v>8.1299000000000007E-3</v>
       </c>
-      <c r="E45">
+      <c r="E47">
         <v>0.1517</v>
       </c>
-      <c r="K45" t="s">
+      <c r="K47" t="s">
         <v>16</v>
       </c>
-      <c r="L45" t="s">
+      <c r="L47" t="s">
         <v>16</v>
       </c>
-      <c r="M45" s="9">
+      <c r="M47" s="8">
         <v>7.2202380000000002</v>
       </c>
-      <c r="N45" s="21">
+      <c r="N47" s="17">
         <v>3.0728829999999999E-2</v>
       </c>
-      <c r="O45" s="21">
+      <c r="O47" s="17">
         <v>0.56113345000000003</v>
       </c>
     </row>

</xml_diff>